<commit_message>
data modified in IPL folder
</commit_message>
<xml_diff>
--- a/webScrapping/espn_scrapper/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
+++ b/webScrapping/espn_scrapper/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,21 +413,27 @@
         <v>result</v>
       </c>
       <c r="D1" t="str">
+        <v>ownTeam</v>
+      </c>
+      <c r="E1" t="str">
+        <v>oppTeam</v>
+      </c>
+      <c r="F1" t="str">
         <v>batsman</v>
       </c>
-      <c r="E1" t="str">
+      <c r="G1" t="str">
         <v>totalRuns</v>
       </c>
-      <c r="F1" t="str">
+      <c r="H1" t="str">
         <v>totalBalls</v>
       </c>
-      <c r="G1" t="str">
+      <c r="I1" t="str">
         <v>total4s</v>
       </c>
-      <c r="H1" t="str">
+      <c r="J1" t="str">
         <v>total6s</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>sr</v>
       </c>
     </row>
@@ -436,120 +442,389 @@
         <v xml:space="preserve"> Abu Dhabi</v>
       </c>
       <c r="B2" t="str">
-        <v xml:space="preserve"> October 19 2020</v>
+        <v xml:space="preserve"> October 07 2020</v>
       </c>
       <c r="C2" t="str">
-        <v>Royals won by 7 wickets (with 15 balls remaining)</v>
+        <v>KKR won by 10 runs</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">Ambati Rayudu </v>
+        <v>Chennai Super Kings</v>
       </c>
       <c r="E2" t="str">
-        <v>13</v>
+        <v>Kolkata Knight Riders</v>
       </c>
       <c r="F2" t="str">
-        <v>19</v>
+        <v xml:space="preserve">Ambati Rayudu </v>
       </c>
       <c r="G2" t="str">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
+        <v>27</v>
+      </c>
+      <c r="I2" t="str">
+        <v>3</v>
+      </c>
+      <c r="J2" t="str">
         <v>0</v>
       </c>
-      <c r="I2" t="str">
-        <v>68.42</v>
+      <c r="K2" t="str">
+        <v>111.11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve"> Dubai (DSC)</v>
+        <v xml:space="preserve"> Sharjah</v>
       </c>
       <c r="B3" t="str">
-        <v xml:space="preserve"> October 13 2020</v>
+        <v xml:space="preserve"> October 23 2020</v>
       </c>
       <c r="C3" t="str">
-        <v>Super Kings won by 20 runs</v>
+        <v>Mumbai won by 10 wickets (with 46 balls remaining)</v>
       </c>
       <c r="D3" t="str">
-        <v xml:space="preserve">Ambati Rayudu </v>
+        <v>Chennai Super Kings</v>
       </c>
       <c r="E3" t="str">
-        <v>41</v>
+        <v>Mumbai Indians</v>
       </c>
       <c r="F3" t="str">
-        <v>34</v>
+        <v xml:space="preserve">Ambati Rayudu </v>
       </c>
       <c r="G3" t="str">
+        <v>2</v>
+      </c>
+      <c r="H3" t="str">
         <v>3</v>
       </c>
-      <c r="H3" t="str">
-        <v>2</v>
-      </c>
       <c r="I3" t="str">
-        <v>120.58</v>
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <v>0</v>
+      </c>
+      <c r="K3" t="str">
+        <v>66.66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve"> Sharjah</v>
+        <v xml:space="preserve"> Abu Dhabi</v>
       </c>
       <c r="B4" t="str">
-        <v xml:space="preserve"> October 17 2020</v>
+        <v xml:space="preserve"> November 01 2020</v>
       </c>
       <c r="C4" t="str">
-        <v>Capitals won by 5 wickets (with 1 ball remaining)</v>
+        <v>Super Kings won by 9 wickets (with 7 balls remaining)</v>
       </c>
       <c r="D4" t="str">
-        <v xml:space="preserve">Ambati Rayudu </v>
+        <v>Chennai Super Kings</v>
       </c>
       <c r="E4" t="str">
-        <v>45</v>
+        <v>Kings XI Punjab</v>
       </c>
       <c r="F4" t="str">
-        <v>25</v>
+        <v xml:space="preserve">Ambati Rayudu </v>
       </c>
       <c r="G4" t="str">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I4" t="str">
-        <v>180.00</v>
+        <v>2</v>
+      </c>
+      <c r="J4" t="str">
+        <v>0</v>
+      </c>
+      <c r="K4" t="str">
+        <v>100.00</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve"> October 13 2020</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Super Kings won by 20 runs</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Sunrisers Hyderabad</v>
+      </c>
+      <c r="F5" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G5" t="str">
+        <v>41</v>
+      </c>
+      <c r="H5" t="str">
+        <v>34</v>
+      </c>
+      <c r="I5" t="str">
+        <v>3</v>
+      </c>
+      <c r="J5" t="str">
+        <v>2</v>
+      </c>
+      <c r="K5" t="str">
+        <v>120.58</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
         <v xml:space="preserve"> Sharjah</v>
       </c>
-      <c r="B5" t="str">
-        <v xml:space="preserve"> October 23 2020</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Mumbai won by 10 wickets (with 46 balls remaining)</v>
-      </c>
-      <c r="D5" t="str">
-        <v xml:space="preserve">Ambati Rayudu </v>
-      </c>
-      <c r="E5" t="str">
+      <c r="B6" t="str">
+        <v xml:space="preserve"> October 17 2020</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Capitals won by 5 wickets (with 1 ball remaining)</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="F6" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G6" t="str">
+        <v>45</v>
+      </c>
+      <c r="H6" t="str">
+        <v>25</v>
+      </c>
+      <c r="I6" t="str">
+        <v>1</v>
+      </c>
+      <c r="J6" t="str">
+        <v>4</v>
+      </c>
+      <c r="K6" t="str">
+        <v>180.00</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve"> September 19 2020</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Super Kings won by 5 wickets (with 4 balls remaining)</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="F7" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G7" t="str">
+        <v>71</v>
+      </c>
+      <c r="H7" t="str">
+        <v>48</v>
+      </c>
+      <c r="I7" t="str">
+        <v>6</v>
+      </c>
+      <c r="J7" t="str">
+        <v>3</v>
+      </c>
+      <c r="K7" t="str">
+        <v>147.91</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="B8" t="str">
+        <v xml:space="preserve"> October 19 2020</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Royals won by 7 wickets (with 15 balls remaining)</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Rajasthan Royals</v>
+      </c>
+      <c r="F8" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G8" t="str">
+        <v>13</v>
+      </c>
+      <c r="H8" t="str">
+        <v>19</v>
+      </c>
+      <c r="I8" t="str">
         <v>2</v>
       </c>
-      <c r="F5" t="str">
+      <c r="J8" t="str">
+        <v>0</v>
+      </c>
+      <c r="K8" t="str">
+        <v>68.42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B9" t="str">
+        <v xml:space="preserve"> October 29 2020</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Super Kings won by 6 wickets</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Kolkata Knight Riders</v>
+      </c>
+      <c r="F9" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G9" t="str">
+        <v>38</v>
+      </c>
+      <c r="H9" t="str">
+        <v>20</v>
+      </c>
+      <c r="I9" t="str">
+        <v>5</v>
+      </c>
+      <c r="J9" t="str">
+        <v>1</v>
+      </c>
+      <c r="K9" t="str">
+        <v>190.00</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B10" t="str">
+        <v xml:space="preserve"> October 02 2020</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Sunrisers won by 7 runs</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Sunrisers Hyderabad</v>
+      </c>
+      <c r="F10" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G10" t="str">
+        <v>8</v>
+      </c>
+      <c r="H10" t="str">
+        <v>9</v>
+      </c>
+      <c r="I10" t="str">
+        <v>1</v>
+      </c>
+      <c r="J10" t="str">
+        <v>0</v>
+      </c>
+      <c r="K10" t="str">
+        <v>88.88</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B11" t="str">
+        <v xml:space="preserve"> October 25 2020</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Super Kings won by 8 wickets (with 8 balls remaining)</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Royal Challengers Bangalore</v>
+      </c>
+      <c r="F11" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G11" t="str">
+        <v>39</v>
+      </c>
+      <c r="H11" t="str">
+        <v>27</v>
+      </c>
+      <c r="I11" t="str">
         <v>3</v>
       </c>
-      <c r="G5" t="str">
+      <c r="J11" t="str">
+        <v>2</v>
+      </c>
+      <c r="K11" t="str">
+        <v>144.44</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B12" t="str">
+        <v xml:space="preserve"> October 10 2020</v>
+      </c>
+      <c r="C12" t="str">
+        <v>RCB won by 37 runs</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Royal Challengers Bangalore</v>
+      </c>
+      <c r="F12" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G12" t="str">
+        <v>42</v>
+      </c>
+      <c r="H12" t="str">
+        <v>40</v>
+      </c>
+      <c r="I12" t="str">
+        <v>4</v>
+      </c>
+      <c r="J12" t="str">
         <v>0</v>
       </c>
-      <c r="H5" t="str">
-        <v>0</v>
-      </c>
-      <c r="I5" t="str">
-        <v>66.66</v>
+      <c r="K12" t="str">
+        <v>105.00</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
json file code updated
</commit_message>
<xml_diff>
--- a/webScrapping/espn_scrapper/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
+++ b/webScrapping/espn_scrapper/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -822,9 +822,394 @@
         <v>100.00</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B13" t="str">
+        <v xml:space="preserve"> October 13 2020</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Super Kings won by 20 runs</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Sunrisers Hyderabad</v>
+      </c>
+      <c r="F13" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G13" t="str">
+        <v>41</v>
+      </c>
+      <c r="H13" t="str">
+        <v>34</v>
+      </c>
+      <c r="I13" t="str">
+        <v>3</v>
+      </c>
+      <c r="J13" t="str">
+        <v>2</v>
+      </c>
+      <c r="K13" t="str">
+        <v>120.58</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="B14" t="str">
+        <v xml:space="preserve"> September 19 2020</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Super Kings won by 5 wickets (with 4 balls remaining)</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="F14" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G14" t="str">
+        <v>71</v>
+      </c>
+      <c r="H14" t="str">
+        <v>48</v>
+      </c>
+      <c r="I14" t="str">
+        <v>6</v>
+      </c>
+      <c r="J14" t="str">
+        <v>3</v>
+      </c>
+      <c r="K14" t="str">
+        <v>147.91</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B15" t="str">
+        <v xml:space="preserve"> October 25 2020</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Super Kings won by 8 wickets (with 8 balls remaining)</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Royal Challengers Bangalore</v>
+      </c>
+      <c r="F15" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G15" t="str">
+        <v>39</v>
+      </c>
+      <c r="H15" t="str">
+        <v>27</v>
+      </c>
+      <c r="I15" t="str">
+        <v>3</v>
+      </c>
+      <c r="J15" t="str">
+        <v>2</v>
+      </c>
+      <c r="K15" t="str">
+        <v>144.44</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v xml:space="preserve"> Sharjah</v>
+      </c>
+      <c r="B16" t="str">
+        <v xml:space="preserve"> October 23 2020</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Mumbai won by 10 wickets (with 46 balls remaining)</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Mumbai Indians</v>
+      </c>
+      <c r="F16" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G16" t="str">
+        <v>2</v>
+      </c>
+      <c r="H16" t="str">
+        <v>3</v>
+      </c>
+      <c r="I16" t="str">
+        <v>0</v>
+      </c>
+      <c r="J16" t="str">
+        <v>0</v>
+      </c>
+      <c r="K16" t="str">
+        <v>66.66</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="B17" t="str">
+        <v xml:space="preserve"> November 01 2020</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Super Kings won by 9 wickets (with 7 balls remaining)</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Kings XI Punjab</v>
+      </c>
+      <c r="F17" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G17" t="str">
+        <v>30</v>
+      </c>
+      <c r="H17" t="str">
+        <v>30</v>
+      </c>
+      <c r="I17" t="str">
+        <v>2</v>
+      </c>
+      <c r="J17" t="str">
+        <v>0</v>
+      </c>
+      <c r="K17" t="str">
+        <v>100.00</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B18" t="str">
+        <v xml:space="preserve"> October 02 2020</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Sunrisers won by 7 runs</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Sunrisers Hyderabad</v>
+      </c>
+      <c r="F18" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G18" t="str">
+        <v>8</v>
+      </c>
+      <c r="H18" t="str">
+        <v>9</v>
+      </c>
+      <c r="I18" t="str">
+        <v>1</v>
+      </c>
+      <c r="J18" t="str">
+        <v>0</v>
+      </c>
+      <c r="K18" t="str">
+        <v>88.88</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B19" t="str">
+        <v xml:space="preserve"> October 29 2020</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Super Kings won by 6 wickets</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Kolkata Knight Riders</v>
+      </c>
+      <c r="F19" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G19" t="str">
+        <v>38</v>
+      </c>
+      <c r="H19" t="str">
+        <v>20</v>
+      </c>
+      <c r="I19" t="str">
+        <v>5</v>
+      </c>
+      <c r="J19" t="str">
+        <v>1</v>
+      </c>
+      <c r="K19" t="str">
+        <v>190.00</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v xml:space="preserve"> Sharjah</v>
+      </c>
+      <c r="B20" t="str">
+        <v xml:space="preserve"> October 17 2020</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Capitals won by 5 wickets (with 1 ball remaining)</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Delhi Capitals</v>
+      </c>
+      <c r="F20" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G20" t="str">
+        <v>45</v>
+      </c>
+      <c r="H20" t="str">
+        <v>25</v>
+      </c>
+      <c r="I20" t="str">
+        <v>1</v>
+      </c>
+      <c r="J20" t="str">
+        <v>4</v>
+      </c>
+      <c r="K20" t="str">
+        <v>180.00</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="B21" t="str">
+        <v xml:space="preserve"> October 19 2020</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Royals won by 7 wickets (with 15 balls remaining)</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Rajasthan Royals</v>
+      </c>
+      <c r="F21" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G21" t="str">
+        <v>13</v>
+      </c>
+      <c r="H21" t="str">
+        <v>19</v>
+      </c>
+      <c r="I21" t="str">
+        <v>2</v>
+      </c>
+      <c r="J21" t="str">
+        <v>0</v>
+      </c>
+      <c r="K21" t="str">
+        <v>68.42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v xml:space="preserve"> Dubai (DSC)</v>
+      </c>
+      <c r="B22" t="str">
+        <v xml:space="preserve"> October 10 2020</v>
+      </c>
+      <c r="C22" t="str">
+        <v>RCB won by 37 runs</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Royal Challengers Bangalore</v>
+      </c>
+      <c r="F22" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G22" t="str">
+        <v>42</v>
+      </c>
+      <c r="H22" t="str">
+        <v>40</v>
+      </c>
+      <c r="I22" t="str">
+        <v>4</v>
+      </c>
+      <c r="J22" t="str">
+        <v>0</v>
+      </c>
+      <c r="K22" t="str">
+        <v>105.00</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v xml:space="preserve"> Abu Dhabi</v>
+      </c>
+      <c r="B23" t="str">
+        <v xml:space="preserve"> October 07 2020</v>
+      </c>
+      <c r="C23" t="str">
+        <v>KKR won by 10 runs</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Kolkata Knight Riders</v>
+      </c>
+      <c r="F23" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="G23" t="str">
+        <v>30</v>
+      </c>
+      <c r="H23" t="str">
+        <v>27</v>
+      </c>
+      <c r="I23" t="str">
+        <v>3</v>
+      </c>
+      <c r="J23" t="str">
+        <v>0</v>
+      </c>
+      <c r="K23" t="str">
+        <v>111.11</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>